<commit_message>
Wybór wstrząsu i ładne okienko wybrania pliku.
</commit_message>
<xml_diff>
--- a/miler.xlsx
+++ b/miler.xlsx
@@ -177,7 +177,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -228,20 +228,9 @@
       <c r="D2" s="0" t="n">
         <v>-600</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="1"/>
+      <c r="G2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>6951</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>3222</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>6955</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>3223</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -257,20 +246,9 @@
       <c r="D3" s="0" t="n">
         <v>-800</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="1"/>
+      <c r="G3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>7023</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>3896</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>7029</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>3905</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -286,20 +264,9 @@
       <c r="D4" s="0" t="n">
         <v>-400</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="1"/>
+      <c r="G4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>7054</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>4011</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>7055</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>4004</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -315,20 +282,9 @@
       <c r="D5" s="0" t="n">
         <v>-1000</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="1"/>
+      <c r="G5" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>6991</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>3636</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>6982</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>3627</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -344,20 +300,9 @@
       <c r="D6" s="0" t="n">
         <v>-1000</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="1"/>
+      <c r="G6" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>6893</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>3780</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>6904</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <v>3780</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -373,20 +318,9 @@
       <c r="D7" s="0" t="n">
         <v>-200</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="1"/>
+      <c r="G7" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>6863</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>3396</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>6964</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <v>3391</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -402,20 +336,9 @@
       <c r="D8" s="0" t="n">
         <v>-600</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="1"/>
+      <c r="G8" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>7052</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>3815</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <v>7041</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>3809</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -431,20 +354,9 @@
       <c r="D9" s="0" t="n">
         <v>-200</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="1"/>
+      <c r="G9" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="G9" s="0" t="n">
-        <v>7135</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>4061</v>
-      </c>
-      <c r="I9" s="0" t="n">
-        <v>7135</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <v>4071</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>